<commit_message>
fix cell string &&  add example && readme
</commit_message>
<xml_diff>
--- a/tests/template-excel/sample-string-output.xlsx
+++ b/tests/template-excel/sample-string-output.xlsx
@@ -17,25 +17,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>{C1}</t>
-  </si>
-  <si>
-    <t>{D1}</t>
-  </si>
-  <si>
-    <t>hi a2</t>
-  </si>
-  <si>
-    <t>hello c2 -</t>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>{unmatchedType}</t>
+  </si>
+  <si>
+    <t>{undefined}</t>
+  </si>
+  <si>
+    <t>i am a2!</t>
   </si>
   <si>
     <t>nice day</t>
+  </si>
+  <si>
+    <t>lyy love lzy</t>
   </si>
 </sst>
 </file>
@@ -371,13 +371,19 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15" customWidth="true" style="0"/>
+    <col min="3" max="3" width="17.6640625" customWidth="true" style="0"/>
+    <col min="4" max="4" width="11.77734375" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -400,18 +406,36 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2"/>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6"/>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>